<commit_message>
increase the value of gold
</commit_message>
<xml_diff>
--- a/planning/country pop balance.xlsx
+++ b/planning/country pop balance.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13050" windowHeight="11655" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="resources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="140">
   <si>
     <t>Country Name</t>
   </si>
@@ -295,6 +296,150 @@
   </si>
   <si>
     <t>zlobenia</t>
+  </si>
+  <si>
+    <t>supply</t>
+  </si>
+  <si>
+    <t>demand</t>
+  </si>
+  <si>
+    <t>cotton</t>
+  </si>
+  <si>
+    <t>dye</t>
+  </si>
+  <si>
+    <t>wool</t>
+  </si>
+  <si>
+    <t>silk</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>sulphur</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>timber</t>
+  </si>
+  <si>
+    <t>tropical</t>
+  </si>
+  <si>
+    <t>rubber</t>
+  </si>
+  <si>
+    <t>clay</t>
+  </si>
+  <si>
+    <t>pearwood</t>
+  </si>
+  <si>
+    <t>steel</t>
+  </si>
+  <si>
+    <t>cement</t>
+  </si>
+  <si>
+    <t>machine parts</t>
+  </si>
+  <si>
+    <t>glass</t>
+  </si>
+  <si>
+    <t>fertiliser</t>
+  </si>
+  <si>
+    <t>boats</t>
+  </si>
+  <si>
+    <t>fabric</t>
+  </si>
+  <si>
+    <t>lumber</t>
+  </si>
+  <si>
+    <t>re-annual</t>
+  </si>
+  <si>
+    <t>treacle</t>
+  </si>
+  <si>
+    <t>brassicas</t>
+  </si>
+  <si>
+    <t>fats</t>
+  </si>
+  <si>
+    <t>paper</t>
+  </si>
+  <si>
+    <t>cattle</t>
+  </si>
+  <si>
+    <t>fish</t>
+  </si>
+  <si>
+    <t>fruit</t>
+  </si>
+  <si>
+    <t>wheat</t>
+  </si>
+  <si>
+    <t>tobacco</t>
+  </si>
+  <si>
+    <t>tea</t>
+  </si>
+  <si>
+    <t>coffee</t>
+  </si>
+  <si>
+    <t>drugs</t>
+  </si>
+  <si>
+    <t>wine</t>
+  </si>
+  <si>
+    <t>liquor</t>
+  </si>
+  <si>
+    <t>clothes</t>
+  </si>
+  <si>
+    <t>luxury clothes</t>
+  </si>
+  <si>
+    <t>furniture</t>
+  </si>
+  <si>
+    <t>luxury Furniture</t>
+  </si>
+  <si>
+    <t>vul wine</t>
+  </si>
+  <si>
+    <t>ceramics</t>
+  </si>
+  <si>
+    <t>swords</t>
+  </si>
+  <si>
+    <t>spears</t>
+  </si>
+  <si>
+    <t>armor</t>
+  </si>
+  <si>
+    <t>siege</t>
+  </si>
+  <si>
+    <t>demand weight</t>
   </si>
 </sst>
 </file>
@@ -604,7 +749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -614,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,4 +1224,715 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" t="s">
+        <v>103</v>
+      </c>
+      <c r="L1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2">
+        <v>132.83600000000001</v>
+      </c>
+      <c r="C2">
+        <v>10.337</v>
+      </c>
+      <c r="D2">
+        <v>56.695999999999998</v>
+      </c>
+      <c r="E2">
+        <v>11.582000000000001</v>
+      </c>
+      <c r="F2">
+        <v>196.15899999999999</v>
+      </c>
+      <c r="G2">
+        <v>13.448</v>
+      </c>
+      <c r="H2">
+        <v>81.224000000000004</v>
+      </c>
+      <c r="I2">
+        <v>1587.51</v>
+      </c>
+      <c r="J2">
+        <v>43.981000000000002</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>87.183999999999997</v>
+      </c>
+      <c r="M2">
+        <v>1.5660000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3">
+        <v>264.81299999999999</v>
+      </c>
+      <c r="C3">
+        <v>37.241</v>
+      </c>
+      <c r="D3">
+        <v>55.625999999999998</v>
+      </c>
+      <c r="E3">
+        <v>33.917000000000002</v>
+      </c>
+      <c r="F3">
+        <v>360.86399999999998</v>
+      </c>
+      <c r="G3">
+        <v>31.466999999999999</v>
+      </c>
+      <c r="H3">
+        <v>123.36</v>
+      </c>
+      <c r="I3">
+        <v>1356.7170000000001</v>
+      </c>
+      <c r="J3">
+        <v>95.512</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>58.970999999999997</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B4">
+        <f>SUM(B2/B3)</f>
+        <v>0.50162189922700173</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:M4" si="0">SUM(C2/C3)</f>
+        <v>0.27757041969871915</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1.0192356092474741</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>0.34148067340861515</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.5435815154739736</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="0"/>
+        <v>0.42736835414879082</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0.65843060959792477</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>1.1701113791601343</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0.46047617053354556</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>1.4784215970561803</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="0"/>
+        <v>1.5660000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>106</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="s">
+        <v>111</v>
+      </c>
+      <c r="H6" t="s">
+        <v>112</v>
+      </c>
+      <c r="I6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7">
+        <v>60.923000000000002</v>
+      </c>
+      <c r="C7">
+        <v>25.286999999999999</v>
+      </c>
+      <c r="D7">
+        <v>3.5569999999999999</v>
+      </c>
+      <c r="E7">
+        <v>115.98399999999999</v>
+      </c>
+      <c r="F7">
+        <v>6.7720000000000002</v>
+      </c>
+      <c r="G7">
+        <v>4.5940000000000003</v>
+      </c>
+      <c r="H7">
+        <v>190.42400000000001</v>
+      </c>
+      <c r="I7">
+        <v>602.39700000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B8">
+        <v>47.96</v>
+      </c>
+      <c r="C8">
+        <v>17.617999999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.7430000000000001</v>
+      </c>
+      <c r="E8">
+        <v>79.832999999999998</v>
+      </c>
+      <c r="F8">
+        <v>13.936</v>
+      </c>
+      <c r="G8">
+        <v>4.5940000000000003</v>
+      </c>
+      <c r="H8">
+        <v>713.69200000000001</v>
+      </c>
+      <c r="I8">
+        <v>453.95499999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>139</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B7/B8)</f>
+        <v>1.2702877397831527</v>
+      </c>
+      <c r="C9">
+        <f t="shared" ref="C9:I9" si="1">SUM(C7/C8)</f>
+        <v>1.4352934498808039</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.0407343660355708</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>1.4528327884458807</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="1"/>
+        <v>0.48593570608495984</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>0.26681537694131363</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>1.3269971693229508</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+      <c r="E10" t="s">
+        <v>117</v>
+      </c>
+      <c r="F10" t="s">
+        <v>118</v>
+      </c>
+      <c r="G10" t="s">
+        <v>119</v>
+      </c>
+      <c r="H10" t="s">
+        <v>120</v>
+      </c>
+      <c r="I10" t="s">
+        <v>121</v>
+      </c>
+      <c r="J10" t="s">
+        <v>122</v>
+      </c>
+      <c r="K10" t="s">
+        <v>123</v>
+      </c>
+      <c r="L10" t="s">
+        <v>124</v>
+      </c>
+      <c r="M10" t="s">
+        <v>125</v>
+      </c>
+      <c r="N10" t="s">
+        <v>126</v>
+      </c>
+      <c r="O10" t="s">
+        <v>127</v>
+      </c>
+      <c r="P10" t="s">
+        <v>128</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>129</v>
+      </c>
+      <c r="R10" t="s">
+        <v>130</v>
+      </c>
+      <c r="S10" t="s">
+        <v>131</v>
+      </c>
+      <c r="T10" t="s">
+        <v>132</v>
+      </c>
+      <c r="U10" t="s">
+        <v>133</v>
+      </c>
+      <c r="V10" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B11">
+        <v>1.8029999999999999</v>
+      </c>
+      <c r="C11">
+        <v>13.362</v>
+      </c>
+      <c r="D11">
+        <v>50.423000000000002</v>
+      </c>
+      <c r="E11">
+        <v>22.916</v>
+      </c>
+      <c r="F11">
+        <v>170.364</v>
+      </c>
+      <c r="G11">
+        <v>50.38</v>
+      </c>
+      <c r="H11">
+        <v>69.103999999999999</v>
+      </c>
+      <c r="I11">
+        <v>59.262999999999998</v>
+      </c>
+      <c r="J11">
+        <v>181.833</v>
+      </c>
+      <c r="K11">
+        <v>95.682000000000002</v>
+      </c>
+      <c r="L11">
+        <v>53.362000000000002</v>
+      </c>
+      <c r="M11">
+        <v>21.117000000000001</v>
+      </c>
+      <c r="N11">
+        <v>4.16</v>
+      </c>
+      <c r="O11">
+        <v>18.774999999999999</v>
+      </c>
+      <c r="P11">
+        <v>122.35299999999999</v>
+      </c>
+      <c r="Q11">
+        <v>250.88300000000001</v>
+      </c>
+      <c r="R11">
+        <v>6.016</v>
+      </c>
+      <c r="S11">
+        <v>287.108</v>
+      </c>
+      <c r="T11">
+        <v>6.7729999999999997</v>
+      </c>
+      <c r="U11">
+        <v>3.073</v>
+      </c>
+      <c r="V11">
+        <v>114.241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B12">
+        <v>1.167</v>
+      </c>
+      <c r="C12">
+        <v>10.955</v>
+      </c>
+      <c r="D12">
+        <v>48.898000000000003</v>
+      </c>
+      <c r="E12">
+        <v>31.89</v>
+      </c>
+      <c r="F12">
+        <v>172.14599999999999</v>
+      </c>
+      <c r="G12">
+        <v>76.539000000000001</v>
+      </c>
+      <c r="H12">
+        <v>51.715000000000003</v>
+      </c>
+      <c r="I12">
+        <v>64.298000000000002</v>
+      </c>
+      <c r="J12">
+        <v>271.41699999999997</v>
+      </c>
+      <c r="K12">
+        <v>157.91900000000001</v>
+      </c>
+      <c r="L12">
+        <v>184.292</v>
+      </c>
+      <c r="M12">
+        <v>98.156000000000006</v>
+      </c>
+      <c r="N12">
+        <v>14.292</v>
+      </c>
+      <c r="O12">
+        <v>143.80600000000001</v>
+      </c>
+      <c r="P12">
+        <v>376.58199999999999</v>
+      </c>
+      <c r="Q12">
+        <v>538.85599999999999</v>
+      </c>
+      <c r="R12">
+        <v>13.938000000000001</v>
+      </c>
+      <c r="S12">
+        <v>533.22400000000005</v>
+      </c>
+      <c r="T12">
+        <v>13.938000000000001</v>
+      </c>
+      <c r="U12">
+        <v>1.4570000000000001</v>
+      </c>
+      <c r="V12">
+        <v>204.53899999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+      <c r="B13">
+        <f>SUM(B11/B12)</f>
+        <v>1.5449871465295628</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:V13" si="2">SUM(C11/C12)</f>
+        <v>1.2197170241898676</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>1.0311873696265696</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="2"/>
+        <v>0.7185951708999686</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="2"/>
+        <v>0.98964832177337847</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>0.65822652503952239</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="2"/>
+        <v>1.3362467369235231</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="2"/>
+        <v>0.92169274316463956</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="2"/>
+        <v>0.66993961321508977</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0.60589289445855155</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>0.28955136413951771</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="2"/>
+        <v>0.21513712865234932</v>
+      </c>
+      <c r="N13">
+        <f t="shared" si="2"/>
+        <v>0.29107192835152534</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="2"/>
+        <v>0.13055783486085418</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="2"/>
+        <v>0.32490400497102889</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" si="2"/>
+        <v>0.46558449752809661</v>
+      </c>
+      <c r="R13">
+        <f t="shared" si="2"/>
+        <v>0.43162577127277946</v>
+      </c>
+      <c r="S13">
+        <f t="shared" si="2"/>
+        <v>0.53843787976535185</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="2"/>
+        <v>0.48593772420720327</v>
+      </c>
+      <c r="U13">
+        <f t="shared" si="2"/>
+        <v>2.109128345916266</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="2"/>
+        <v>0.55852918025413245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>135</v>
+      </c>
+      <c r="C14" t="s">
+        <v>136</v>
+      </c>
+      <c r="D14" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15">
+        <v>14.478999999999999</v>
+      </c>
+      <c r="C15">
+        <v>9.8979999999999997</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>2.14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16">
+        <v>8.9459999999999997</v>
+      </c>
+      <c r="C16">
+        <v>8.1969999999999992</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>139</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B15/B16)</f>
+        <v>1.6184887100380059</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:E17" si="3">SUM(C15/C16)</f>
+        <v>1.2075149444918873</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>2.14</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B4:M4 B13:V13 B9:I9 B17:E17">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <cfvo type="num" val="2"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF92D050"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{5B6FA066-661F-4F78-8F4A-38A281605584}">
+            <x14:iconSet iconSet="3Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>33</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent" gte="0">
+                <xm:f>67</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3ArrowsGray" iconId="2"/>
+              <x14:cfIcon iconSet="3Triangles" iconId="1"/>
+              <x14:cfIcon iconSet="3ArrowsGray" iconId="0"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>B4:M4 B13:V13 B9:I9 B17:E17</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>